<commit_message>
Rename Folder_SubFolder association to SubFolder_Folder
</commit_message>
<xml_diff>
--- a/static/originals/refguide/query-over-example-database.xlsx
+++ b/static/originals/refguide/query-over-example-database.xlsx
@@ -1,11 +1,11 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22430"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26227"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{182D548D-6380-41F2-8516-12B91606B207}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{63B0EA9C-A4DD-4962-BD08-98E27EDE4069}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-156" yWindow="-156" windowWidth="31032" windowHeight="16992" xr2:uid="{C59F0884-246F-40F7-AE73-1B2F573881EA}"/>
+    <workbookView xWindow="1710" yWindow="-19890" windowWidth="28800" windowHeight="15105" xr2:uid="{C59F0884-246F-40F7-AE73-1B2F573881EA}"/>
   </bookViews>
   <sheets>
     <sheet name="Query Over Folders" sheetId="1" r:id="rId1"/>
@@ -66,7 +66,7 @@
     <t>ParentFolderID</t>
   </si>
   <si>
-    <t>Folder_SubFolder</t>
+    <t>SubFolder_Folder</t>
   </si>
 </sst>
 </file>
@@ -500,27 +500,27 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{467C0ABE-6991-4525-B249-23D043470656}">
   <dimension ref="B2:K29"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A11" workbookViewId="0">
-      <selection activeCell="C26" sqref="C26"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A34" sqref="A34"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.86328125" defaultRowHeight="13.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultColWidth="8.81640625" defaultRowHeight="14" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="8.86328125" style="1"/>
-    <col min="2" max="2" width="2.9296875" style="1" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="17.1328125" style="4" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="11.9296875" style="1" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="8.86328125" style="1"/>
-    <col min="6" max="6" width="13.9296875" style="1" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="15.3984375" style="1" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="8.86328125" style="1" customWidth="1"/>
-    <col min="9" max="9" width="2.9296875" style="1" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="17.1328125" style="1" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="11.9296875" style="1" bestFit="1" customWidth="1"/>
-    <col min="12" max="16384" width="8.86328125" style="1"/>
+    <col min="1" max="1" width="8.81640625" style="1"/>
+    <col min="2" max="2" width="2.90625" style="1" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="17.08984375" style="4" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="11.90625" style="1" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="8.81640625" style="1"/>
+    <col min="6" max="6" width="13.90625" style="1" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="15.36328125" style="1" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="8.81640625" style="1" customWidth="1"/>
+    <col min="9" max="9" width="2.90625" style="1" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="17.08984375" style="1" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="11.90625" style="1" bestFit="1" customWidth="1"/>
+    <col min="12" max="16384" width="8.81640625" style="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:11" x14ac:dyDescent="0.35">
+    <row r="2" spans="2:11" x14ac:dyDescent="0.3">
       <c r="B2" s="5" t="s">
         <v>0</v>
       </c>
@@ -537,7 +537,7 @@
       <c r="J2" s="6"/>
       <c r="K2" s="5"/>
     </row>
-    <row r="3" spans="2:11" x14ac:dyDescent="0.35">
+    <row r="3" spans="2:11" x14ac:dyDescent="0.3">
       <c r="B3" s="8" t="s">
         <v>1</v>
       </c>
@@ -564,7 +564,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="4" spans="2:11" x14ac:dyDescent="0.35">
+    <row r="4" spans="2:11" x14ac:dyDescent="0.3">
       <c r="B4" s="2">
         <v>1</v>
       </c>
@@ -590,7 +590,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="5" spans="2:11" x14ac:dyDescent="0.35">
+    <row r="5" spans="2:11" x14ac:dyDescent="0.3">
       <c r="B5" s="2">
         <v>2</v>
       </c>
@@ -616,7 +616,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="6" spans="2:11" x14ac:dyDescent="0.35">
+    <row r="6" spans="2:11" x14ac:dyDescent="0.3">
       <c r="B6" s="2">
         <v>3</v>
       </c>
@@ -642,7 +642,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="7" spans="2:11" x14ac:dyDescent="0.35">
+    <row r="7" spans="2:11" x14ac:dyDescent="0.3">
       <c r="B7" s="2">
         <v>4</v>
       </c>
@@ -668,7 +668,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="8" spans="2:11" x14ac:dyDescent="0.35">
+    <row r="8" spans="2:11" x14ac:dyDescent="0.3">
       <c r="B8" s="2">
         <v>5</v>
       </c>
@@ -694,7 +694,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="9" spans="2:11" x14ac:dyDescent="0.35">
+    <row r="9" spans="2:11" x14ac:dyDescent="0.3">
       <c r="B9" s="2">
         <v>6</v>
       </c>
@@ -714,7 +714,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="12" spans="2:11" x14ac:dyDescent="0.35">
+    <row r="12" spans="2:11" x14ac:dyDescent="0.3">
       <c r="B12" s="5" t="s">
         <v>0</v>
       </c>
@@ -731,7 +731,7 @@
       <c r="J12" s="6"/>
       <c r="K12" s="5"/>
     </row>
-    <row r="13" spans="2:11" x14ac:dyDescent="0.35">
+    <row r="13" spans="2:11" x14ac:dyDescent="0.3">
       <c r="B13" s="8" t="s">
         <v>1</v>
       </c>
@@ -758,7 +758,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="14" spans="2:11" x14ac:dyDescent="0.35">
+    <row r="14" spans="2:11" x14ac:dyDescent="0.3">
       <c r="B14" s="2">
         <v>1</v>
       </c>
@@ -784,7 +784,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="15" spans="2:11" x14ac:dyDescent="0.35">
+    <row r="15" spans="2:11" x14ac:dyDescent="0.3">
       <c r="B15" s="2">
         <v>2</v>
       </c>
@@ -810,7 +810,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="16" spans="2:11" x14ac:dyDescent="0.35">
+    <row r="16" spans="2:11" x14ac:dyDescent="0.3">
       <c r="B16" s="2">
         <v>3</v>
       </c>
@@ -836,7 +836,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="17" spans="2:11" x14ac:dyDescent="0.35">
+    <row r="17" spans="2:11" x14ac:dyDescent="0.3">
       <c r="B17" s="2">
         <v>4</v>
       </c>
@@ -862,7 +862,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="18" spans="2:11" x14ac:dyDescent="0.35">
+    <row r="18" spans="2:11" x14ac:dyDescent="0.3">
       <c r="B18" s="12">
         <v>5</v>
       </c>
@@ -888,7 +888,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="19" spans="2:11" x14ac:dyDescent="0.35">
+    <row r="19" spans="2:11" x14ac:dyDescent="0.3">
       <c r="B19" s="12">
         <v>6</v>
       </c>
@@ -908,7 +908,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="22" spans="2:11" x14ac:dyDescent="0.35">
+    <row r="22" spans="2:11" x14ac:dyDescent="0.3">
       <c r="B22" s="5" t="s">
         <v>0</v>
       </c>
@@ -925,7 +925,7 @@
       <c r="J22" s="6"/>
       <c r="K22" s="5"/>
     </row>
-    <row r="23" spans="2:11" x14ac:dyDescent="0.35">
+    <row r="23" spans="2:11" x14ac:dyDescent="0.3">
       <c r="B23" s="8" t="s">
         <v>1</v>
       </c>
@@ -952,7 +952,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="24" spans="2:11" x14ac:dyDescent="0.35">
+    <row r="24" spans="2:11" x14ac:dyDescent="0.3">
       <c r="B24" s="2">
         <v>1</v>
       </c>
@@ -978,7 +978,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="25" spans="2:11" x14ac:dyDescent="0.35">
+    <row r="25" spans="2:11" x14ac:dyDescent="0.3">
       <c r="B25" s="2">
         <v>2</v>
       </c>
@@ -1004,7 +1004,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="26" spans="2:11" x14ac:dyDescent="0.35">
+    <row r="26" spans="2:11" x14ac:dyDescent="0.3">
       <c r="B26" s="12">
         <v>3</v>
       </c>
@@ -1030,7 +1030,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="27" spans="2:11" x14ac:dyDescent="0.35">
+    <row r="27" spans="2:11" x14ac:dyDescent="0.3">
       <c r="B27" s="2">
         <v>4</v>
       </c>
@@ -1056,7 +1056,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="28" spans="2:11" x14ac:dyDescent="0.35">
+    <row r="28" spans="2:11" x14ac:dyDescent="0.3">
       <c r="B28" s="2">
         <v>5</v>
       </c>
@@ -1082,7 +1082,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="29" spans="2:11" x14ac:dyDescent="0.35">
+    <row r="29" spans="2:11" x14ac:dyDescent="0.3">
       <c r="B29" s="2">
         <v>6</v>
       </c>

</xml_diff>